<commit_message>
Dosyalar son kez çalışıldı ve güncellendi
</commit_message>
<xml_diff>
--- a/maas.xlsx
+++ b/maas.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
   <si>
     <t>TL ÖZEL CARİ HESAP</t>
   </si>
@@ -39,12 +39,6 @@
     <t>Kullanılabilir Bakiye</t>
   </si>
   <si>
-    <t>74-1809273-4/ISPARTA ŞUBESİ</t>
-  </si>
-  <si>
-    <t>TR22 0020 3000 0180 9273 0000 04</t>
-  </si>
-  <si>
     <t>TL Cari Hesap</t>
   </si>
   <si>
@@ -63,12 +57,6 @@
     <t>Vade Tarihi</t>
   </si>
   <si>
-    <t>74-1809273-2/ISPARTA ŞUBESİ</t>
-  </si>
-  <si>
-    <t>TR76 0020 3000 0180 9273 0000 02</t>
-  </si>
-  <si>
     <t>Katılma Hesabı</t>
   </si>
   <si>
@@ -78,16 +66,19 @@
     <t>1 Ay</t>
   </si>
   <si>
-    <t>1,982.92 USD</t>
-  </si>
-  <si>
-    <t>74-1809273-5/ISPARTA ŞUBESİ</t>
-  </si>
-  <si>
-    <t>TR92 0020 3000 0180 9273 0000 05</t>
-  </si>
-  <si>
-    <t>9,762.92 EUR</t>
+    <t>97-1818181-4/QQQ ŞUBESİ</t>
+  </si>
+  <si>
+    <t>TRQQ 0020 3000 0180 YYYY 0000 OO</t>
+  </si>
+  <si>
+    <t>97-1818181-5/QQQ ŞUBESİ</t>
+  </si>
+  <si>
+    <t>50 USD</t>
+  </si>
+  <si>
+    <t>50 EUR</t>
   </si>
 </sst>
 </file>
@@ -589,7 +580,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -606,10 +597,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -935,7 +929,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11:F12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -971,33 +967,33 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="C3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>10</v>
+      <c r="E3" s="8" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
+        <v>16</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1011,83 +1007,77 @@
         <v>3</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="E9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="6">
+        <v>42180</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="7">
-        <v>42180</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="6"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="5" t="s">
+      <c r="A11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="6">
+        <v>42180</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" s="7">
-        <v>42180</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
@@ -1096,6 +1086,12 @@
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>